<commit_message>
correction of 04 data file
</commit_message>
<xml_diff>
--- a/q1_dataFiles/04_Wahrscheinlichkeitsverteilungen.xlsx
+++ b/q1_dataFiles/04_Wahrscheinlichkeitsverteilungen.xlsx
@@ -1,43 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\engelmann6\Dropbox\QuantiWebsite\q1_dataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B345CE4C-A7A5-4024-BD40-239AADE53324}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="997" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="997" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binomialverteilung_1_Aufgabe" sheetId="10" r:id="rId1"/>
     <sheet name="Binomialverteilung_1_Lösung" sheetId="11" r:id="rId2"/>
     <sheet name="Binomialverteilung 2 Aufgabe" sheetId="12" r:id="rId3"/>
-    <sheet name="Binomialverteilung 2 Lösung" sheetId="9" r:id="rId4"/>
+    <sheet name="Binomialverteilung 2 Lösung NEU" sheetId="14" r:id="rId4"/>
     <sheet name="Normalverteilung_Aufgabe" sheetId="13" r:id="rId5"/>
     <sheet name="Normalverteilung_Lösung" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="72">
   <si>
     <t>Anzahl richtige Antworten</t>
   </si>
@@ -251,11 +244,14 @@
   <si>
     <t>Das Kriterium müsste "mindestens 18 richtige Antworten" lauten.</t>
   </si>
+  <si>
+    <t>p(k =&lt; 58|unfair)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -495,6 +491,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -557,7 +556,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1293,7 +1292,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1331,7 +1330,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="548568936"/>
@@ -1413,7 +1412,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1445,7 +1444,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="548574512"/>
@@ -1486,7 +1485,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1537,7 +1536,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2274,7 +2273,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2312,7 +2311,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461191976"/>
@@ -2394,7 +2393,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2426,7 +2425,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="461189680"/>
@@ -2467,7 +2466,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2548,7 +2547,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3626,7 +3625,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3664,7 +3663,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="636606632"/>
@@ -3746,7 +3745,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3778,7 +3777,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="636608272"/>
@@ -3819,7 +3818,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3870,7 +3869,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4590,7 +4589,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="555404008"/>
@@ -4649,7 +4648,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="555411552"/>
@@ -4690,7 +4689,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4746,7 +4745,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4772,7 +4770,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4788,7 +4786,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Binomialverteilung 2 Lösung'!$B$25</c:f>
+              <c:f>'Binomialverteilung 2 Lösung NEU'!$B$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4809,7 +4807,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Binomialverteilung 2 Lösung'!$A$26:$A$51</c:f>
+              <c:f>'Binomialverteilung 2 Lösung NEU'!$A$26:$A$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -4896,7 +4894,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Binomialverteilung 2 Lösung'!$B$26:$B$51</c:f>
+              <c:f>'Binomialverteilung 2 Lösung NEU'!$B$26:$B$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -4983,7 +4981,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3649-46CE-A183-79F60318801C}"/>
+              <c16:uniqueId val="{00000000-F1C7-4A85-89F4-B2A9AC405F04}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4992,7 +4990,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Binomialverteilung 2 Lösung'!$E$25</c:f>
+              <c:f>'Binomialverteilung 2 Lösung NEU'!$F$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5013,7 +5011,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Binomialverteilung 2 Lösung'!$E$26:$E$51</c:f>
+              <c:f>'Binomialverteilung 2 Lösung NEU'!$F$26:$F$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -5100,7 +5098,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3649-46CE-A183-79F60318801C}"/>
+              <c16:uniqueId val="{00000001-F1C7-4A85-89F4-B2A9AC405F04}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5150,7 +5148,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5176,7 +5173,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5214,7 +5211,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="451517664"/>
@@ -5271,7 +5268,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5297,7 +5293,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5329,7 +5325,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="451516024"/>
@@ -5370,7 +5366,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5446,7 +5442,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6063,7 +6059,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6101,7 +6097,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="636950040"/>
@@ -6153,7 +6149,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Wahrscheinlichkeit</a:t>
+                  <a:t>Wahrscheinlichkeitsdichte</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6183,7 +6179,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6215,7 +6211,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="636953648"/>
@@ -6256,7 +6252,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6332,7 +6328,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6949,7 +6945,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6961,10 +6957,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -6987,7 +6980,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="554368032"/>
@@ -7001,6 +6994,7 @@
         <c:axId val="554368032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7069,7 +7063,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7080,7 +7074,9 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -7101,7 +7097,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="554375904"/>
@@ -7142,7 +7138,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11026,7 +11022,7 @@
         <xdr:cNvPr id="2" name="Grafik 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{088471EF-5104-40AA-84CB-DB3AADB83E07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11041,7 +11037,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{837473B0-CC2E-450A-ABE3-18F120FF3D39}">
-              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" xmlns="" r:id="rId2"/>
+              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" r:id="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -11076,7 +11072,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Wolkenförmige Legende 2"/>
+        <xdr:cNvPr id="3" name="Wolkenförmige Legende 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11138,7 +11140,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Grafik 10"/>
+        <xdr:cNvPr id="11" name="Grafik 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11187,7 +11195,7 @@
         <xdr:cNvPr id="2" name="Grafik 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{088471EF-5104-40AA-84CB-DB3AADB83E07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11202,7 +11210,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{837473B0-CC2E-450A-ABE3-18F120FF3D39}">
-              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" xmlns="" r:id="rId2"/>
+              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" r:id="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -11224,20 +11232,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>752474</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
+      <xdr:colOff>276224</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11269,7 +11283,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvPr id="4" name="Diagramm 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11301,7 +11321,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvPr id="5" name="Diagramm 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11333,7 +11359,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Diagramm 5"/>
+        <xdr:cNvPr id="6" name="Diagramm 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11365,7 +11397,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Ovale Legende 6"/>
+        <xdr:cNvPr id="7" name="Ovale Legende 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11427,7 +11465,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Textfeld 7"/>
+        <xdr:cNvPr id="8" name="Textfeld 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11511,7 +11555,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Grafik 8"/>
+        <xdr:cNvPr id="9" name="Grafik 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11559,7 +11609,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1" descr="Smart cat - ForFun"/>
+        <xdr:cNvPr id="2" name="Grafik 1" descr="Smart cat - ForFun">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -11606,20 +11662,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1009650</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>523874</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1" descr="Smart cat - ForFun"/>
+        <xdr:cNvPr id="2" name="Grafik 1" descr="Smart cat - ForFun">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FE456BC-613E-45CF-B8F0-CBBB12771F4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -11639,7 +11701,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8096250" y="0"/>
+          <a:off x="9020175" y="0"/>
           <a:ext cx="1685924" cy="1685924"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -11661,21 +11723,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>390525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B5348CE-FEF9-4196-BC25-20E8A010586C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -11709,7 +11779,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11747,7 +11823,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Wolkenförmige Legende 2"/>
+        <xdr:cNvPr id="3" name="Wolkenförmige Legende 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11809,7 +11891,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Grafik 5"/>
+        <xdr:cNvPr id="6" name="Grafik 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11835,6 +11923,74 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rechteck 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D70FBDF4-F97D-4ECF-AE8B-E981F814ECB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10258425" y="12144375"/>
+          <a:ext cx="2943225" cy="1628775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>=</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -11855,7 +12011,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -11885,7 +12047,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -11920,7 +12088,7 @@
             <xdr14:cNvPr id="4" name="Freihand 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CD86A5A-E86C-4AFE-9CE6-8D332B43FF1F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -11980,7 +12148,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Gerader Verbinder 6"/>
+        <xdr:cNvPr id="7" name="Gerader Verbinder 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -12355,10 +12529,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H136"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -13294,11 +13468,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13648,15 +13822,15 @@
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="8" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="G26" s="8">
-        <f>E91</f>
-        <v>3.9677888294059995E-3</v>
+        <f>E92</f>
+        <v>7.1735625993735374E-3</v>
       </c>
       <c r="H26" s="15">
-        <f>SUM(D34:D91)</f>
-        <v>3.9677888294059969E-3</v>
+        <f>SUM(D34:D92)</f>
+        <v>7.1735625993735192E-3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -13749,11 +13923,11 @@
         <v>7.8886090522101049E-31</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C65" si="0">_xlfn.BINOM.DIST(A34,100,0.5,TRUE)</f>
+        <f>_xlfn.BINOM.DIST(A34,100,0.5,TRUE)</f>
         <v>7.8886090522101049E-31</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D65" si="1">_xlfn.BINOM.DIST(A34,100,0.7,FALSE)</f>
+        <f t="shared" ref="D34:D65" si="0">_xlfn.BINOM.DIST(A34,100,0.7,FALSE)</f>
         <v>5.153775207320163E-53</v>
       </c>
       <c r="E34">
@@ -13766,15 +13940,15 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35:B98" si="2">_xlfn.BINOM.DIST(A35,100,0.5,FALSE)</f>
+        <f t="shared" ref="B35:B98" si="1">_xlfn.BINOM.DIST(A35,100,0.5,FALSE)</f>
         <v>7.8886090522101158E-29</v>
       </c>
       <c r="C35">
+        <f t="shared" ref="C34:C65" si="2">_xlfn.BINOM.DIST(A35,100,0.5,TRUE)</f>
+        <v>7.9674951427322349E-29</v>
+      </c>
+      <c r="D35">
         <f t="shared" si="0"/>
-        <v>7.9674951427322349E-29</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="1"/>
         <v>1.2025475483746942E-50</v>
       </c>
       <c r="E35">
@@ -13787,15 +13961,15 @@
         <v>2</v>
       </c>
       <c r="B36">
+        <f t="shared" si="1"/>
+        <v>3.9048614808440493E-27</v>
+      </c>
+      <c r="C36">
         <f t="shared" si="2"/>
-        <v>3.9048614808440493E-27</v>
-      </c>
-      <c r="C36">
+        <v>3.9845364322713471E-27</v>
+      </c>
+      <c r="D36">
         <f t="shared" si="0"/>
-        <v>3.9845364322713471E-27</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="1"/>
         <v>1.3889424183727732E-48</v>
       </c>
       <c r="E36">
@@ -13808,15 +13982,15 @@
         <v>3</v>
       </c>
       <c r="B37">
+        <f t="shared" si="1"/>
+        <v>1.2755880837423889E-25</v>
+      </c>
+      <c r="C37">
         <f t="shared" si="2"/>
-        <v>1.2755880837423889E-25</v>
-      </c>
-      <c r="C37">
+        <v>1.315433448065097E-25</v>
+      </c>
+      <c r="D37">
         <f t="shared" si="0"/>
-        <v>1.315433448065097E-25</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="1"/>
         <v>1.0586827766707993E-46</v>
       </c>
       <c r="E37">
@@ -13829,15 +14003,15 @@
         <v>4</v>
       </c>
       <c r="B38">
+        <f t="shared" si="1"/>
+        <v>3.0933011030752918E-24</v>
+      </c>
+      <c r="C38">
         <f t="shared" si="2"/>
-        <v>3.0933011030752918E-24</v>
-      </c>
-      <c r="C38">
+        <v>3.2248444478817956E-24</v>
+      </c>
+      <c r="D38">
         <f t="shared" si="0"/>
-        <v>3.2248444478817956E-24</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="1"/>
         <v>5.9903800446623789E-45</v>
       </c>
       <c r="E38">
@@ -13850,15 +14024,15 @@
         <v>5</v>
       </c>
       <c r="B39">
+        <f t="shared" si="1"/>
+        <v>5.9391381179045101E-23</v>
+      </c>
+      <c r="C39">
         <f t="shared" si="2"/>
-        <v>5.9391381179045101E-23</v>
-      </c>
-      <c r="C39">
+        <v>6.2616225626926508E-23</v>
+      </c>
+      <c r="D39">
         <f t="shared" si="0"/>
-        <v>6.2616225626926508E-23</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="1"/>
         <v>2.6836902600087162E-43</v>
       </c>
       <c r="E39">
@@ -13871,15 +14045,15 @@
         <v>6</v>
       </c>
       <c r="B40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9.4036353533488793E-22</v>
       </c>
       <c r="C40">
+        <f>_xlfn.BINOM.DIST(A40,100,0.5,TRUE)</f>
+        <v>1.0029797609618036E-21</v>
+      </c>
+      <c r="D40">
         <f t="shared" si="0"/>
-        <v>1.0029797609618036E-21</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="1"/>
         <v>9.9147445716989156E-42</v>
       </c>
       <c r="E40">
@@ -13892,15 +14066,15 @@
         <v>7</v>
       </c>
       <c r="B41">
+        <f t="shared" si="1"/>
+        <v>1.2627738903068301E-20</v>
+      </c>
+      <c r="C41">
         <f t="shared" si="2"/>
-        <v>1.2627738903068301E-20</v>
-      </c>
-      <c r="C41">
+        <v>1.3630718664030184E-20</v>
+      </c>
+      <c r="D41">
         <f t="shared" si="0"/>
-        <v>1.3630718664030184E-20</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="1"/>
         <v>3.1066199657989591E-40</v>
       </c>
       <c r="E41">
@@ -13913,15 +14087,15 @@
         <v>8</v>
       </c>
       <c r="B42">
+        <f t="shared" si="1"/>
+        <v>1.4679746474816979E-19</v>
+      </c>
+      <c r="C42">
         <f t="shared" si="2"/>
-        <v>1.4679746474816979E-19</v>
-      </c>
-      <c r="C42">
+        <v>1.6042818341220037E-19</v>
+      </c>
+      <c r="D42">
         <f t="shared" si="0"/>
-        <v>1.6042818341220037E-19</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="1"/>
         <v>8.4267066572298191E-39</v>
       </c>
       <c r="E42">
@@ -13934,15 +14108,15 @@
         <v>9</v>
       </c>
       <c r="B43">
+        <f t="shared" si="1"/>
+        <v>1.5005963063146118E-18</v>
+      </c>
+      <c r="C43">
         <f t="shared" si="2"/>
-        <v>1.5005963063146118E-18</v>
-      </c>
-      <c r="C43">
+        <v>1.6610244897268311E-18</v>
+      </c>
+      <c r="D43">
         <f t="shared" si="0"/>
-        <v>1.6610244897268311E-18</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="1"/>
         <v>2.0099255878725997E-37</v>
       </c>
       <c r="E43">
@@ -13955,15 +14129,15 @@
         <v>10</v>
       </c>
       <c r="B44">
+        <f t="shared" si="1"/>
+        <v>1.3655426387462979E-17</v>
+      </c>
+      <c r="C44">
         <f t="shared" si="2"/>
-        <v>1.3655426387462979E-17</v>
-      </c>
-      <c r="C44">
+        <v>1.531645087719E-17</v>
+      </c>
+      <c r="D44">
         <f t="shared" si="0"/>
-        <v>1.531645087719E-17</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="1"/>
         <v>4.2677419982495376E-36</v>
       </c>
       <c r="E44">
@@ -13976,15 +14150,15 @@
         <v>11</v>
       </c>
       <c r="B45">
+        <f t="shared" si="1"/>
+        <v>1.1172621589742489E-16</v>
+      </c>
+      <c r="C45">
         <f t="shared" si="2"/>
-        <v>1.1172621589742489E-16</v>
-      </c>
-      <c r="C45">
+        <v>1.2704266677461521E-16</v>
+      </c>
+      <c r="D45">
         <f t="shared" si="0"/>
-        <v>1.2704266677461521E-16</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="1"/>
         <v>8.1475074512034476E-35</v>
       </c>
       <c r="E45">
@@ -13997,15 +14171,15 @@
         <v>12</v>
       </c>
       <c r="B46">
+        <f t="shared" si="1"/>
+        <v>8.2863610123923984E-16</v>
+      </c>
+      <c r="C46">
         <f t="shared" si="2"/>
-        <v>8.2863610123923984E-16</v>
-      </c>
-      <c r="C46">
+        <v>9.5567876801385473E-16</v>
+      </c>
+      <c r="D46">
         <f t="shared" si="0"/>
-        <v>9.5567876801385473E-16</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="1"/>
         <v>1.4099714283610658E-33</v>
       </c>
       <c r="E46">
@@ -14018,15 +14192,15 @@
         <v>13</v>
       </c>
       <c r="B47">
+        <f t="shared" si="1"/>
+        <v>5.6092289930040794E-15</v>
+      </c>
+      <c r="C47">
         <f t="shared" si="2"/>
-        <v>5.6092289930040794E-15</v>
-      </c>
-      <c r="C47">
+        <v>6.5649077610179485E-15</v>
+      </c>
+      <c r="D47">
         <f t="shared" si="0"/>
-        <v>6.5649077610179485E-15</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="1"/>
         <v>2.2270317945395133E-32</v>
       </c>
       <c r="E47">
@@ -14039,15 +14213,15 @@
         <v>14</v>
       </c>
       <c r="B48">
+        <f t="shared" si="1"/>
+        <v>3.4857351599382189E-14</v>
+      </c>
+      <c r="C48">
         <f t="shared" si="2"/>
-        <v>3.4857351599382189E-14</v>
-      </c>
-      <c r="C48">
+        <v>4.1422259360400582E-14</v>
+      </c>
+      <c r="D48">
         <f t="shared" si="0"/>
-        <v>4.1422259360400582E-14</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="1"/>
         <v>3.2291961020822452E-31</v>
       </c>
       <c r="E48">
@@ -14060,15 +14234,15 @@
         <v>15</v>
       </c>
       <c r="B49">
+        <f t="shared" si="1"/>
+        <v>1.9984881583645948E-13</v>
+      </c>
+      <c r="C49">
         <f t="shared" si="2"/>
-        <v>1.9984881583645948E-13</v>
-      </c>
-      <c r="C49">
+        <v>2.4127107519685985E-13</v>
+      </c>
+      <c r="D49">
         <f t="shared" si="0"/>
-        <v>2.4127107519685985E-13</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="1"/>
         <v>4.3199467854523319E-30</v>
       </c>
       <c r="E49">
@@ -14081,15 +14255,15 @@
         <v>16</v>
       </c>
       <c r="B50">
+        <f t="shared" si="1"/>
+        <v>1.0616968341311918E-12</v>
+      </c>
+      <c r="C50">
         <f t="shared" si="2"/>
-        <v>1.0616968341311918E-12</v>
-      </c>
-      <c r="C50">
+        <v>1.3029679093280532E-12</v>
+      </c>
+      <c r="D50">
         <f t="shared" si="0"/>
-        <v>1.3029679093280532E-12</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="1"/>
         <v>5.3549340361335903E-29</v>
       </c>
       <c r="E50">
@@ -14102,15 +14276,15 @@
         <v>17</v>
       </c>
       <c r="B51">
+        <f t="shared" si="1"/>
+        <v>5.2460314157070423E-12</v>
+      </c>
+      <c r="C51">
         <f t="shared" si="2"/>
-        <v>5.2460314157070423E-12</v>
-      </c>
-      <c r="C51">
+        <v>6.5489993250351334E-12</v>
+      </c>
+      <c r="D51">
         <f t="shared" si="0"/>
-        <v>6.5489993250351334E-12</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="1"/>
         <v>6.1739239475422777E-28</v>
       </c>
       <c r="E51">
@@ -14123,15 +14297,15 @@
         <v>18</v>
       </c>
       <c r="B52">
+        <f t="shared" si="1"/>
+        <v>2.419003375020489E-11</v>
+      </c>
+      <c r="C52">
         <f t="shared" si="2"/>
-        <v>2.419003375020489E-11</v>
-      </c>
-      <c r="C52">
+        <v>3.0739033075240051E-11</v>
+      </c>
+      <c r="D52">
         <f t="shared" si="0"/>
-        <v>3.0739033075240051E-11</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="1"/>
         <v>6.6426848398556367E-27</v>
       </c>
       <c r="E52">
@@ -14144,15 +14318,15 @@
         <v>19</v>
       </c>
       <c r="B53">
+        <f t="shared" si="1"/>
+        <v>1.0439909302719939E-10</v>
+      </c>
+      <c r="C53">
         <f t="shared" si="2"/>
-        <v>1.0439909302719939E-10</v>
-      </c>
-      <c r="C53">
+        <v>1.3513812610243952E-10</v>
+      </c>
+      <c r="D53">
         <f t="shared" si="0"/>
-        <v>1.3513812610243952E-10</v>
-      </c>
-      <c r="D53">
-        <f t="shared" si="1"/>
         <v>6.6893001720651607E-26</v>
       </c>
       <c r="E53">
@@ -14165,15 +14339,15 @@
         <v>20</v>
       </c>
       <c r="B54">
+        <f t="shared" si="1"/>
+        <v>4.2281632676015464E-10</v>
+      </c>
+      <c r="C54">
         <f t="shared" si="2"/>
-        <v>4.2281632676015464E-10</v>
-      </c>
-      <c r="C54">
+        <v>5.5795445286259861E-10</v>
+      </c>
+      <c r="D54">
         <f t="shared" si="0"/>
-        <v>5.5795445286259861E-10</v>
-      </c>
-      <c r="D54">
-        <f t="shared" si="1"/>
         <v>6.3213886626015146E-25</v>
       </c>
       <c r="E54">
@@ -14186,15 +14360,15 @@
         <v>21</v>
       </c>
       <c r="B55">
+        <f t="shared" si="1"/>
+        <v>1.6107288638482146E-9</v>
+      </c>
+      <c r="C55">
         <f t="shared" si="2"/>
-        <v>1.6107288638482146E-9</v>
-      </c>
-      <c r="C55">
+        <v>2.1686833167108283E-9</v>
+      </c>
+      <c r="D55">
         <f t="shared" si="0"/>
-        <v>2.1686833167108283E-9</v>
-      </c>
-      <c r="D55">
-        <f t="shared" si="1"/>
         <v>5.6190121445347262E-24</v>
       </c>
       <c r="E55">
@@ -14207,15 +14381,15 @@
         <v>22</v>
       </c>
       <c r="B56">
+        <f t="shared" si="1"/>
+        <v>5.7839809201822048E-9</v>
+      </c>
+      <c r="C56">
         <f t="shared" si="2"/>
-        <v>5.7839809201822048E-9</v>
-      </c>
-      <c r="C56">
+        <v>7.95266423689306E-9</v>
+      </c>
+      <c r="D56">
         <f t="shared" si="0"/>
-        <v>7.95266423689306E-9</v>
-      </c>
-      <c r="D56">
-        <f t="shared" si="1"/>
         <v>4.7080510847389326E-23</v>
       </c>
       <c r="E56">
@@ -14228,15 +14402,15 @@
         <v>23</v>
       </c>
       <c r="B57">
+        <f t="shared" si="1"/>
+        <v>1.9615239642357071E-8</v>
+      </c>
+      <c r="C57">
         <f t="shared" si="2"/>
-        <v>1.9615239642357071E-8</v>
-      </c>
-      <c r="C57">
+        <v>2.756790387925027E-8</v>
+      </c>
+      <c r="D57">
         <f t="shared" si="0"/>
-        <v>2.756790387925027E-8</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="1"/>
         <v>3.7255012931412435E-22</v>
       </c>
       <c r="E57">
@@ -14249,15 +14423,15 @@
         <v>24</v>
       </c>
       <c r="B58">
+        <f t="shared" si="1"/>
+        <v>6.2932227185896111E-8</v>
+      </c>
+      <c r="C58">
         <f t="shared" si="2"/>
-        <v>6.2932227185896111E-8</v>
-      </c>
-      <c r="C58">
+        <v>9.0500131065146477E-8</v>
+      </c>
+      <c r="D58">
         <f t="shared" si="0"/>
-        <v>9.0500131065146477E-8</v>
-      </c>
-      <c r="D58">
-        <f t="shared" si="1"/>
         <v>2.7889516625043276E-21</v>
       </c>
       <c r="E58">
@@ -14270,15 +14444,15 @@
         <v>25</v>
       </c>
       <c r="B59">
+        <f t="shared" si="1"/>
+        <v>1.9131397064512392E-7</v>
+      </c>
+      <c r="C59">
         <f t="shared" si="2"/>
-        <v>1.9131397064512392E-7</v>
-      </c>
-      <c r="C59">
+        <v>2.8181410171027133E-7</v>
+      </c>
+      <c r="D59">
         <f t="shared" si="0"/>
-        <v>2.8181410171027133E-7</v>
-      </c>
-      <c r="D59">
-        <f t="shared" si="1"/>
         <v>1.9782963792697521E-20</v>
       </c>
       <c r="E59">
@@ -14291,15 +14465,15 @@
         <v>26</v>
       </c>
       <c r="B60">
+        <f t="shared" si="1"/>
+        <v>5.5186722301477995E-7</v>
+      </c>
+      <c r="C60">
         <f t="shared" si="2"/>
-        <v>5.5186722301477995E-7</v>
-      </c>
-      <c r="C60">
+        <v>8.336813247250498E-7</v>
+      </c>
+      <c r="D60">
         <f t="shared" si="0"/>
-        <v>8.336813247250498E-7</v>
-      </c>
-      <c r="D60">
-        <f t="shared" si="1"/>
         <v>1.3315456398931022E-19</v>
       </c>
       <c r="E60">
@@ -14312,15 +14486,15 @@
         <v>27</v>
       </c>
       <c r="B61">
+        <f t="shared" si="1"/>
+        <v>1.5125249815960639E-6</v>
+      </c>
+      <c r="C61">
         <f t="shared" si="2"/>
-        <v>1.5125249815960639E-6</v>
-      </c>
-      <c r="C61">
+        <v>2.3462063063211181E-6</v>
+      </c>
+      <c r="D61">
         <f t="shared" si="0"/>
-        <v>2.3462063063211181E-6</v>
-      </c>
-      <c r="D61">
-        <f t="shared" si="1"/>
         <v>8.5153165612915941E-19</v>
       </c>
       <c r="E61">
@@ -14333,15 +14507,15 @@
         <v>28</v>
       </c>
       <c r="B62">
+        <f t="shared" si="1"/>
+        <v>3.9433687020183031E-6</v>
+      </c>
+      <c r="C62">
         <f t="shared" si="2"/>
-        <v>3.9433687020183031E-6</v>
-      </c>
-      <c r="C62">
+        <v>6.2895750083394441E-6</v>
+      </c>
+      <c r="D62">
         <f t="shared" si="0"/>
-        <v>6.2895750083394441E-6</v>
-      </c>
-      <c r="D62">
-        <f t="shared" si="1"/>
         <v>5.1801509081190473E-18</v>
       </c>
       <c r="E62">
@@ -14354,15 +14528,15 @@
         <v>29</v>
       </c>
       <c r="B63">
+        <f t="shared" si="1"/>
+        <v>9.7904326394937912E-6</v>
+      </c>
+      <c r="C63">
         <f t="shared" si="2"/>
-        <v>9.7904326394937912E-6</v>
-      </c>
-      <c r="C63">
+        <v>1.6080007647833249E-5</v>
+      </c>
+      <c r="D63">
         <f t="shared" si="0"/>
-        <v>1.6080007647833249E-5</v>
-      </c>
-      <c r="D63">
-        <f t="shared" si="1"/>
         <v>3.0009150088414038E-17</v>
       </c>
       <c r="E63">
@@ -14375,15 +14549,15 @@
         <v>30</v>
       </c>
       <c r="B64">
+        <f t="shared" si="1"/>
+        <v>2.3170690580135296E-5</v>
+      </c>
+      <c r="C64">
         <f t="shared" si="2"/>
-        <v>2.3170690580135296E-5</v>
-      </c>
-      <c r="C64">
+        <v>3.9250698227968307E-5</v>
+      </c>
+      <c r="D64">
         <f t="shared" si="0"/>
-        <v>3.9250698227968307E-5</v>
-      </c>
-      <c r="D64">
-        <f t="shared" si="1"/>
         <v>1.657171954882429E-16</v>
       </c>
       <c r="E64">
@@ -14396,15 +14570,15 @@
         <v>31</v>
       </c>
       <c r="B65">
+        <f t="shared" si="1"/>
+        <v>5.2320914213208622E-5</v>
+      </c>
+      <c r="C65">
         <f t="shared" si="2"/>
-        <v>5.2320914213208622E-5</v>
-      </c>
-      <c r="C65">
+        <v>9.1571612441176896E-5</v>
+      </c>
+      <c r="D65">
         <f t="shared" si="0"/>
-        <v>9.1571612441176896E-5</v>
-      </c>
-      <c r="D65">
-        <f t="shared" si="1"/>
         <v>8.7313361063697608E-16</v>
       </c>
       <c r="E65">
@@ -14417,7 +14591,7 @@
         <v>32</v>
       </c>
       <c r="B66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.1281697127223065E-4</v>
       </c>
       <c r="C66">
@@ -14438,7 +14612,7 @@
         <v>33</v>
       </c>
       <c r="B67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.3247133474277876E-4</v>
       </c>
       <c r="C67">
@@ -14459,7 +14633,7 @@
         <v>34</v>
       </c>
       <c r="B68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.5810527728724036E-4</v>
       </c>
       <c r="C68">
@@ -14480,7 +14654,7 @@
         <v>35</v>
       </c>
       <c r="B69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8.6385566574165252E-4</v>
       </c>
       <c r="C69">
@@ -14501,7 +14675,7 @@
         <v>36</v>
       </c>
       <c r="B70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5597393964779853E-3</v>
       </c>
       <c r="C70">
@@ -14522,7 +14696,7 @@
         <v>37</v>
       </c>
       <c r="B71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.6979276047186741E-3</v>
       </c>
       <c r="C71">
@@ -14543,7 +14717,7 @@
         <v>38</v>
       </c>
       <c r="B72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.4728799762441106E-3</v>
       </c>
       <c r="C72">
@@ -14564,7 +14738,7 @@
         <v>39</v>
       </c>
       <c r="B73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.1107322699265549E-3</v>
       </c>
       <c r="C73">
@@ -14585,7 +14759,7 @@
         <v>40</v>
       </c>
       <c r="B74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.0843866711637992E-2</v>
       </c>
       <c r="C74">
@@ -14606,7 +14780,7 @@
         <v>41</v>
       </c>
       <c r="B75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5869073236543376E-2</v>
       </c>
       <c r="C75">
@@ -14627,7 +14801,7 @@
         <v>42</v>
       </c>
       <c r="B76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.2292269546572856E-2</v>
       </c>
       <c r="C76">
@@ -14648,7 +14822,7 @@
         <v>43</v>
       </c>
       <c r="B77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.0068642644214549E-2</v>
       </c>
       <c r="C77">
@@ -14669,7 +14843,7 @@
         <v>44</v>
       </c>
       <c r="B78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.8952559789096154E-2</v>
       </c>
       <c r="C78">
@@ -14690,7 +14864,7 @@
         <v>45</v>
       </c>
       <c r="B79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.8474296626430782E-2</v>
       </c>
       <c r="C79">
@@ -14711,7 +14885,7 @@
         <v>46</v>
       </c>
       <c r="B80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.7958398140297657E-2</v>
       </c>
       <c r="C80">
@@ -14732,7 +14906,7 @@
         <v>47</v>
       </c>
       <c r="B81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.659049999098024E-2</v>
       </c>
       <c r="C81">
@@ -14753,7 +14927,7 @@
         <v>48</v>
       </c>
       <c r="B82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.3527010406707352E-2</v>
       </c>
       <c r="C82">
@@ -14774,7 +14948,7 @@
         <v>49</v>
       </c>
       <c r="B83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.802866410507725E-2</v>
       </c>
       <c r="C83">
@@ -14795,7 +14969,7 @@
         <v>50</v>
       </c>
       <c r="B84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.9589237387178782E-2</v>
       </c>
       <c r="C84">
@@ -14816,7 +14990,7 @@
         <v>51</v>
       </c>
       <c r="B85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.802866410507725E-2</v>
       </c>
       <c r="C85">
@@ -14837,7 +15011,7 @@
         <v>52</v>
       </c>
       <c r="B86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.3527010406707352E-2</v>
       </c>
       <c r="C86">
@@ -14858,7 +15032,7 @@
         <v>53</v>
       </c>
       <c r="B87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.659049999098024E-2</v>
       </c>
       <c r="C87">
@@ -14879,7 +15053,7 @@
         <v>54</v>
       </c>
       <c r="B88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5.7958398140297643E-2</v>
       </c>
       <c r="C88">
@@ -14900,7 +15074,7 @@
         <v>55</v>
       </c>
       <c r="B89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.8474296626430782E-2</v>
       </c>
       <c r="C89">
@@ -14921,7 +15095,7 @@
         <v>56</v>
       </c>
       <c r="B90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.8952559789096154E-2</v>
       </c>
       <c r="C90">
@@ -14942,7 +15116,7 @@
         <v>57</v>
       </c>
       <c r="B91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.0068642644214549E-2</v>
       </c>
       <c r="C91">
@@ -14963,7 +15137,7 @@
         <v>58</v>
       </c>
       <c r="B92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.2292269546572856E-2</v>
       </c>
       <c r="C92">
@@ -14984,7 +15158,7 @@
         <v>59</v>
       </c>
       <c r="B93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5869073236543376E-2</v>
       </c>
       <c r="C93">
@@ -15005,7 +15179,7 @@
         <v>60</v>
       </c>
       <c r="B94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.0843866711637992E-2</v>
       </c>
       <c r="C94">
@@ -15026,7 +15200,7 @@
         <v>61</v>
       </c>
       <c r="B95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.1107322699265549E-3</v>
       </c>
       <c r="C95">
@@ -15047,7 +15221,7 @@
         <v>62</v>
       </c>
       <c r="B96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.4728799762441098E-3</v>
       </c>
       <c r="C96">
@@ -15068,7 +15242,7 @@
         <v>63</v>
       </c>
       <c r="B97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.6979276047186741E-3</v>
       </c>
       <c r="C97">
@@ -15089,7 +15263,7 @@
         <v>64</v>
       </c>
       <c r="B98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5597393964779846E-3</v>
       </c>
       <c r="C98">
@@ -15869,10 +16043,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -16446,24 +16620,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E7FD7A-42B4-4252-8AD8-B22F1B56FAA2}">
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D51"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
@@ -16479,9 +16653,10 @@
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
-      <c r="N1" s="13"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N1" s="12"/>
+      <c r="O1" s="13"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -16495,9 +16670,10 @@
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
-      <c r="N2" s="15"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N2" s="10"/>
+      <c r="O2" s="15"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -16511,9 +16687,10 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
-      <c r="N3" s="15"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N3" s="10"/>
+      <c r="O3" s="15"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>53</v>
       </c>
@@ -16529,9 +16706,10 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
-      <c r="N4" s="15"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="10"/>
+      <c r="O4" s="15"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -16544,9 +16722,10 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
-      <c r="N5" s="15"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="10"/>
+      <c r="O5" s="15"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>8</v>
       </c>
@@ -16562,9 +16741,10 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="N6" s="15"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="10"/>
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -16578,9 +16758,10 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
-      <c r="N7" s="15"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="10"/>
+      <c r="O7" s="15"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -16594,9 +16775,10 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="15"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="10"/>
+      <c r="O8" s="15"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>9</v>
       </c>
@@ -16612,9 +16794,10 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="15"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N9" s="10"/>
+      <c r="O9" s="15"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>10</v>
       </c>
@@ -16630,9 +16813,10 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="15"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N10" s="10"/>
+      <c r="O10" s="15"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -16646,9 +16830,10 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="15"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="10"/>
+      <c r="O11" s="15"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>54</v>
       </c>
@@ -16660,11 +16845,11 @@
       <c r="D12" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="10"/>
+      <c r="F12" s="8">
         <f>SUM(B41:B51)</f>
         <v>0.21217811107635492</v>
       </c>
-      <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -16672,9 +16857,10 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="15"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="10"/>
+      <c r="O12" s="15"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -16688,9 +16874,10 @@
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="15"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="10"/>
+      <c r="O13" s="15"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>35</v>
       </c>
@@ -16706,9 +16893,10 @@
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="15"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="10"/>
+      <c r="O14" s="15"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -16722,9 +16910,10 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="15"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="10"/>
+      <c r="O15" s="15"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>55</v>
       </c>
@@ -16742,9 +16931,10 @@
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="15"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="10"/>
+      <c r="O16" s="15"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -16758,9 +16948,10 @@
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="15"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N17" s="10"/>
+      <c r="O17" s="15"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>37</v>
       </c>
@@ -16776,9 +16967,10 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
-      <c r="N18" s="15"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N18" s="10"/>
+      <c r="O18" s="15"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -16792,25 +16984,26 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="15"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="10"/>
+      <c r="O19" s="15"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B20" s="8">
-        <f>1-F40</f>
+        <f>1-G40</f>
         <v>2.1451240486669576E-4</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="8">
-        <f>SUM(E41:E51)</f>
+      <c r="E20" s="10"/>
+      <c r="F20" s="8">
+        <f>SUM(F41:F51)</f>
         <v>2.1451240486669614E-4</v>
       </c>
-      <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
@@ -16818,9 +17011,10 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
-      <c r="N20" s="15"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N20" s="10"/>
+      <c r="O20" s="15"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -16834,9 +17028,10 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
-      <c r="N21" s="15"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N21" s="10"/>
+      <c r="O21" s="15"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>38</v>
       </c>
@@ -16852,9 +17047,10 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
-      <c r="N22" s="15"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N22" s="10"/>
+      <c r="O22" s="15"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
@@ -16868,10 +17064,11 @@
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
-      <c r="N23" s="18"/>
-    </row>
-    <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N23" s="17"/>
+      <c r="O23" s="18"/>
+    </row>
+    <row r="24" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>0</v>
       </c>
@@ -16881,20 +17078,21 @@
       <c r="C25" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="34"/>
+      <c r="F25" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="G25" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="21"/>
       <c r="H25" s="21"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I25" s="21"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -16906,23 +17104,27 @@
         <f>_xlfn.BINOM.DIST(A26,25,0.5,TRUE)</f>
         <v>2.9802322387695299E-8</v>
       </c>
-      <c r="D26" t="str">
-        <f>IF(1-C26&lt;=0.05,"ja","nein")</f>
+      <c r="D26">
+        <f>SUM(B26:B$51)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="E26" t="str">
+        <f>IF(D26&lt;=0.05,"ja","nein")</f>
         <v>nein</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <f>_xlfn.BINOM.DIST(A26,25,0.25,FALSE)</f>
         <v>7.5254345816500089E-4</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <f>_xlfn.BINOM.DIST(A26,25,0.25,TRUE)</f>
         <v>7.5254345816500089E-4</v>
       </c>
-      <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -16934,23 +17136,27 @@
         <f t="shared" ref="C27:C51" si="1">_xlfn.BINOM.DIST(A27,25,0.5,TRUE)</f>
         <v>7.7486038208007813E-7</v>
       </c>
-      <c r="D27" t="str">
-        <f t="shared" ref="D27:D51" si="2">IF(1-C27&lt;=0.05,"ja","nein")</f>
+      <c r="D27">
+        <f>SUM(B27:B$51)</f>
+        <v>0.9999999701976775</v>
+      </c>
+      <c r="E27" t="str">
+        <f>IF(D27&lt;=0.05,"ja","nein")</f>
         <v>nein</v>
       </c>
-      <c r="E27">
-        <f t="shared" ref="E27:E51" si="3">_xlfn.BINOM.DIST(A27,25,0.25,FALSE)</f>
+      <c r="F27">
+        <f t="shared" ref="F27:F51" si="2">_xlfn.BINOM.DIST(A27,25,0.25,FALSE)</f>
         <v>6.2711954847083345E-3</v>
       </c>
-      <c r="F27">
-        <f t="shared" ref="F27:F51" si="4">_xlfn.BINOM.DIST(A27,25,0.25,TRUE)</f>
+      <c r="G27">
+        <f t="shared" ref="G27:G51" si="3">_xlfn.BINOM.DIST(A27,25,0.25,TRUE)</f>
         <v>7.0237389428733409E-3</v>
       </c>
-      <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -16962,23 +17168,27 @@
         <f t="shared" si="1"/>
         <v>9.7155570983886702E-6</v>
       </c>
-      <c r="D28" t="str">
+      <c r="D28">
+        <f>SUM(B28:B$51)</f>
+        <v>0.99999922513961781</v>
+      </c>
+      <c r="E28" t="str">
+        <f>IF(D28&lt;=0.05,"ja","nein")</f>
+        <v>nein</v>
+      </c>
+      <c r="F28">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E28">
+        <v>2.5084781938833341E-2</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="3"/>
-        <v>2.5084781938833341E-2</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="4"/>
         <v>3.2108520881706695E-2</v>
       </c>
-      <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -16990,20 +17200,24 @@
         <f t="shared" si="1"/>
         <v>7.8260898590087904E-5</v>
       </c>
-      <c r="D29" t="str">
+      <c r="D29">
+        <f>SUM(B29:B$51)</f>
+        <v>0.9999902844429015</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" ref="E29:E51" si="4">IF(D29&lt;=0.05,"ja","nein")</f>
+        <v>nein</v>
+      </c>
+      <c r="F29">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E29">
+        <v>6.4105553843685228E-2</v>
+      </c>
+      <c r="G29">
         <f t="shared" si="3"/>
-        <v>6.4105553843685228E-2</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="4"/>
         <v>9.6214074725391924E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -17015,20 +17229,24 @@
         <f t="shared" si="1"/>
         <v>4.5526027679443381E-4</v>
       </c>
-      <c r="D30" t="str">
+      <c r="D30">
+        <f>SUM(B30:B$51)</f>
+        <v>0.9999217391014098</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F30">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E30">
+        <v>0.11752684871342284</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="3"/>
-        <v>0.11752684871342284</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="4"/>
         <v>0.21374092343881509</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -17040,20 +17258,24 @@
         <f t="shared" si="1"/>
         <v>2.0386576652526855E-3</v>
       </c>
-      <c r="D31" t="str">
+      <c r="D31">
+        <f>SUM(B31:B$51)</f>
+        <v>0.99954473972320546</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F31">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E31">
+        <v>0.16453758819879205</v>
+      </c>
+      <c r="G31">
         <f t="shared" si="3"/>
-        <v>0.16453758819879205</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="4"/>
         <v>0.37827851163760712</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -17065,20 +17287,24 @@
         <f t="shared" si="1"/>
         <v>7.3166489601135254E-3</v>
       </c>
-      <c r="D32" t="str">
+      <c r="D32">
+        <f>SUM(B32:B$51)</f>
+        <v>0.9979613423347472</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F32">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E32">
+        <v>0.18281954244310228</v>
+      </c>
+      <c r="G32">
         <f t="shared" si="3"/>
-        <v>0.18281954244310228</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="4"/>
         <v>0.5610980540807089</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -17090,20 +17316,24 @@
         <f t="shared" si="1"/>
         <v>2.1642625331878669E-2</v>
       </c>
-      <c r="D33" t="str">
+      <c r="D33">
+        <f>SUM(B33:B$51)</f>
+        <v>0.99268335103988636</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F33">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E33">
+        <v>0.16540815744852111</v>
+      </c>
+      <c r="G33">
         <f t="shared" si="3"/>
-        <v>0.16540815744852111</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="4"/>
         <v>0.72650621152923012</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8</v>
       </c>
@@ -17115,20 +17345,24 @@
         <f t="shared" si="1"/>
         <v>5.3876072168350241E-2</v>
       </c>
-      <c r="D34" t="str">
+      <c r="D34">
+        <f>SUM(B34:B$51)</f>
+        <v>0.97835737466812123</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F34">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E34">
+        <v>0.12405611808639083</v>
+      </c>
+      <c r="G34">
         <f t="shared" si="3"/>
-        <v>0.12405611808639083</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="4"/>
         <v>0.85056232961562084</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
@@ -17140,20 +17374,24 @@
         <f t="shared" si="1"/>
         <v>0.11476147174835211</v>
       </c>
-      <c r="D35" t="str">
+      <c r="D35">
+        <f>SUM(B35:B$51)</f>
+        <v>0.94612392783164978</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F35">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E35">
+        <v>7.8109407684023843E-2</v>
+      </c>
+      <c r="G35">
         <f t="shared" si="3"/>
-        <v>7.8109407684023843E-2</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="4"/>
         <v>0.92867173729964492</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10</v>
       </c>
@@ -17165,20 +17403,24 @@
         <f t="shared" si="1"/>
         <v>0.21217811107635506</v>
       </c>
-      <c r="D36" t="str">
+      <c r="D36">
+        <f>SUM(B36:B$51)</f>
+        <v>0.88523852825164795</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F36">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E36">
+        <v>4.1658350764812689E-2</v>
+      </c>
+      <c r="G36">
         <f t="shared" si="3"/>
-        <v>4.1658350764812689E-2</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="4"/>
         <v>0.97033008806445764</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>11</v>
       </c>
@@ -17190,20 +17432,24 @@
         <f t="shared" si="1"/>
         <v>0.34501898288726823</v>
       </c>
-      <c r="D37" t="str">
+      <c r="D37">
+        <f>SUM(B37:B$51)</f>
+        <v>0.78782188892364502</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F37">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E37">
+        <v>1.8935613984005759E-2</v>
+      </c>
+      <c r="G37">
         <f t="shared" si="3"/>
-        <v>1.8935613984005759E-2</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="4"/>
         <v>0.98926570204846342</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>12</v>
       </c>
@@ -17215,20 +17461,24 @@
         <f t="shared" si="1"/>
         <v>0.49999999999999967</v>
       </c>
-      <c r="D38" t="str">
+      <c r="D38">
+        <f>SUM(B38:B$51)</f>
+        <v>0.65498101711273182</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F38">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E38">
+        <v>7.3638498826689141E-3</v>
+      </c>
+      <c r="G38">
         <f t="shared" si="3"/>
-        <v>7.3638498826689141E-3</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="4"/>
         <v>0.99662955193113234</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>13</v>
       </c>
@@ -17240,20 +17490,24 @@
         <f t="shared" si="1"/>
         <v>0.65498101711273171</v>
       </c>
-      <c r="D39" t="str">
+      <c r="D39">
+        <f>SUM(B39:B$51)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F39">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E39">
+        <v>2.454616627556304E-3</v>
+      </c>
+      <c r="G39">
         <f t="shared" si="3"/>
-        <v>2.454616627556304E-3</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="4"/>
         <v>0.99908416855868865</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>14</v>
       </c>
@@ -17265,20 +17519,24 @@
         <f t="shared" si="1"/>
         <v>0.78782188892364491</v>
       </c>
-      <c r="D40" t="str">
+      <c r="D40">
+        <f>SUM(B40:B$51)</f>
+        <v>0.34501898288726807</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F40">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E40">
+        <v>7.0131903644465876E-4</v>
+      </c>
+      <c r="G40">
         <f t="shared" si="3"/>
-        <v>7.0131903644465876E-4</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="4"/>
         <v>0.9997854875951333</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>15</v>
       </c>
@@ -17290,20 +17548,24 @@
         <f t="shared" si="1"/>
         <v>0.88523852825164795</v>
       </c>
-      <c r="D41" t="str">
+      <c r="D41">
+        <f>SUM(B41:B$51)</f>
+        <v>0.21217811107635492</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F41">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E41">
+        <v>1.714335422420281E-4</v>
+      </c>
+      <c r="G41">
         <f t="shared" si="3"/>
-        <v>1.714335422420281E-4</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="4"/>
         <v>0.99995692113737533</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>16</v>
       </c>
@@ -17315,20 +17577,24 @@
         <f t="shared" si="1"/>
         <v>0.94612392783164978</v>
       </c>
-      <c r="D42" t="str">
+      <c r="D42">
+        <f>SUM(B42:B$51)</f>
+        <v>0.11476147174835201</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F42">
         <f t="shared" si="2"/>
-        <v>nein</v>
-      </c>
-      <c r="E42">
+        <v>3.571532130042237E-5</v>
+      </c>
+      <c r="G42">
         <f t="shared" si="3"/>
-        <v>3.571532130042237E-5</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="4"/>
         <v>0.99999263645867575</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>17</v>
       </c>
@@ -17340,20 +17606,24 @@
         <f t="shared" si="1"/>
         <v>0.97835737466812134</v>
       </c>
-      <c r="D43" t="str">
+      <c r="D43">
+        <f>SUM(B43:B$51)</f>
+        <v>5.3876072168350192E-2</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="4"/>
+        <v>nein</v>
+      </c>
+      <c r="F43">
         <f t="shared" si="2"/>
-        <v>ja</v>
-      </c>
-      <c r="E43">
+        <v>6.3027037588980634E-6</v>
+      </c>
+      <c r="G43">
         <f t="shared" si="3"/>
-        <v>6.3027037588980634E-6</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="4"/>
         <v>0.99999893916243465</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>18</v>
       </c>
@@ -17365,20 +17635,24 @@
         <f t="shared" si="1"/>
         <v>0.99268335103988647</v>
       </c>
-      <c r="D44" t="str">
+      <c r="D44">
+        <f>SUM(B44:B$51)</f>
+        <v>2.1642625331878648E-2</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="4"/>
+        <v>ja</v>
+      </c>
+      <c r="F44">
         <f t="shared" si="2"/>
-        <v>ja</v>
-      </c>
-      <c r="E44">
+        <v>9.3373389020712122E-7</v>
+      </c>
+      <c r="G44">
         <f t="shared" si="3"/>
-        <v>9.3373389020712122E-7</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="4"/>
         <v>0.99999987289632486</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>19</v>
       </c>
@@ -17390,20 +17664,24 @@
         <f t="shared" si="1"/>
         <v>0.99796134233474731</v>
       </c>
-      <c r="D45" t="str">
+      <c r="D45">
+        <f>SUM(B45:B$51)</f>
+        <v>7.3166489601135237E-3</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="4"/>
+        <v>ja</v>
+      </c>
+      <c r="F45">
         <f t="shared" si="2"/>
-        <v>ja</v>
-      </c>
-      <c r="E45">
+        <v>1.146690742359625E-7</v>
+      </c>
+      <c r="G45">
         <f t="shared" si="3"/>
-        <v>1.146690742359625E-7</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="4"/>
         <v>0.9999999875653991</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>20</v>
       </c>
@@ -17415,20 +17693,24 @@
         <f t="shared" si="1"/>
         <v>0.99954473972320557</v>
       </c>
-      <c r="D46" t="str">
+      <c r="D46">
+        <f>SUM(B46:B$51)</f>
+        <v>2.0386576652526829E-3</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="4"/>
+        <v>ja</v>
+      </c>
+      <c r="F46">
         <f t="shared" si="2"/>
-        <v>ja</v>
-      </c>
-      <c r="E46">
+        <v>1.1466907423596243E-8</v>
+      </c>
+      <c r="G46">
         <f t="shared" si="3"/>
-        <v>1.1466907423596243E-8</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="4"/>
         <v>0.99999999903230652</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>21</v>
       </c>
@@ -17440,20 +17722,24 @@
         <f t="shared" si="1"/>
         <v>0.99992173910140991</v>
       </c>
-      <c r="D47" t="str">
+      <c r="D47">
+        <f>SUM(B47:B$51)</f>
+        <v>4.5526027679443349E-4</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="4"/>
+        <v>ja</v>
+      </c>
+      <c r="F47">
         <f t="shared" si="2"/>
-        <v>ja</v>
-      </c>
-      <c r="E47">
+        <v>9.100720177457357E-10</v>
+      </c>
+      <c r="G47">
         <f t="shared" si="3"/>
-        <v>9.100720177457357E-10</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="4"/>
         <v>0.99999999994237854</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>22</v>
       </c>
@@ -17465,20 +17751,24 @@
         <f t="shared" si="1"/>
         <v>0.99999028444290161</v>
       </c>
-      <c r="D48" t="str">
+      <c r="D48">
+        <f>SUM(B48:B$51)</f>
+        <v>7.8260898590087796E-5</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="4"/>
+        <v>ja</v>
+      </c>
+      <c r="F48">
         <f t="shared" si="2"/>
-        <v>ja</v>
-      </c>
-      <c r="E48">
+        <v>5.515587986337799E-11</v>
+      </c>
+      <c r="G48">
         <f t="shared" si="3"/>
-        <v>5.515587986337799E-11</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="4"/>
         <v>0.99999999999753442</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>23</v>
       </c>
@@ -17490,20 +17780,24 @@
         <f t="shared" si="1"/>
         <v>0.99999922513961792</v>
       </c>
-      <c r="D49" t="str">
+      <c r="D49">
+        <f>SUM(B49:B$51)</f>
+        <v>9.7155570983886617E-6</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="4"/>
+        <v>ja</v>
+      </c>
+      <c r="F49">
         <f t="shared" si="2"/>
-        <v>ja</v>
-      </c>
-      <c r="E49">
+        <v>2.3980817331903313E-12</v>
+      </c>
+      <c r="G49">
         <f t="shared" si="3"/>
-        <v>2.3980817331903313E-12</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="4"/>
         <v>0.9999999999999325</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>24</v>
       </c>
@@ -17515,20 +17809,24 @@
         <f t="shared" si="1"/>
         <v>0.99999997019767761</v>
       </c>
-      <c r="D50" t="str">
+      <c r="D50">
+        <f>SUM(B50:B$51)</f>
+        <v>7.7486038208007918E-7</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="4"/>
+        <v>ja</v>
+      </c>
+      <c r="F50">
         <f t="shared" si="2"/>
-        <v>ja</v>
-      </c>
-      <c r="E50">
+        <v>6.6613381477509077E-14</v>
+      </c>
+      <c r="G50">
         <f t="shared" si="3"/>
-        <v>6.6613381477509077E-14</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="4"/>
         <v>0.99999999999999911</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>25</v>
       </c>
@@ -17540,20 +17838,27 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="D51" t="str">
+      <c r="D51">
+        <f>SUM(B51:B$51)</f>
+        <v>2.9802322387695299E-8</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="4"/>
+        <v>ja</v>
+      </c>
+      <c r="F51">
         <f t="shared" si="2"/>
-        <v>ja</v>
-      </c>
-      <c r="E51">
+        <v>8.8817841970012444E-16</v>
+      </c>
+      <c r="G51">
         <f t="shared" si="3"/>
-        <v>8.8817841970012444E-16</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D25:E25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -17561,11 +17866,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17793,8 +18098,14 @@
       <c r="A16">
         <v>60</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="E16" s="4">
+        <f>C26</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <f>740000*E16</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -17839,48 +18150,36 @@
       <c r="A24" s="33">
         <v>68</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
       <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="33">
         <v>69</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
       <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="33">
         <v>70</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
       <c r="D26" s="33"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
         <v>71</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
       <c r="D27" s="33"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="33">
         <v>72</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
       <c r="D28" s="33"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="33">
         <v>73</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
       <c r="D29" s="33"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -18234,11 +18533,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18551,7 +18850,7 @@
         <v>1.7481259395806324E-3</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f>_xlfn.NORM.DIST(A21,100,15,TRUE)</f>
         <v>9.8153286286453353E-3</v>
       </c>
     </row>

</xml_diff>